<commit_message>
names are removed from the results file of user study
</commit_message>
<xml_diff>
--- a/papers/userstudy-results/results.xlsx
+++ b/papers/userstudy-results/results.xlsx
@@ -18,9 +18,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -57,7 +54,10 @@
     <t>?</t>
   </si>
   <si>
-    <t xml:space="preserve"> Mike Collins</t>
+    <t>M. C.</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -532,13 +532,13 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1:M1048576"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="9"/>
-    <col min="2" max="2" width="18.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.140625" style="15" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="16" customWidth="1"/>
     <col min="5" max="5" width="12.140625" style="17" customWidth="1"/>
@@ -552,62 +552,62 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="21" customHeight="1">
       <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="F1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="13" t="s">
+      <c r="I1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="5" customFormat="1" ht="19.5" customHeight="1">
       <c r="A2" s="10"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" customHeight="1">
@@ -615,16 +615,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="16">
         <v>180</v>
       </c>
       <c r="I3" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J3" s="18">
         <v>84</v>
@@ -635,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" s="17">
         <v>3</v>
@@ -693,12 +693,12 @@
     <row r="13" spans="1:10" ht="30" customHeight="1"/>
     <row r="14" spans="1:10" ht="30" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1"/>

</xml_diff>

<commit_message>
user 5 results is added.
</commit_message>
<xml_diff>
--- a/papers/userstudy-results/results.xlsx
+++ b/papers/userstudy-results/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>User</t>
   </si>
@@ -532,7 +532,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O5" sqref="O5:O9"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -674,6 +674,9 @@
       <c r="A6" s="9">
         <v>4</v>
       </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="E6" s="17">
         <v>3</v>
       </c>
@@ -690,6 +693,21 @@
     <row r="7" spans="1:10" ht="30" customHeight="1">
       <c r="A7" s="9">
         <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="15">
+        <v>39</v>
+      </c>
+      <c r="D7" s="16">
+        <v>318</v>
+      </c>
+      <c r="I7" s="17">
+        <v>3</v>
+      </c>
+      <c r="J7" s="18">
+        <v>195</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" customHeight="1">

</xml_diff>